<commit_message>
test material add br
</commit_message>
<xml_diff>
--- a/assets/csv/test1.xlsx
+++ b/assets/csv/test1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>product_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -145,10 +145,6 @@
 ● Octopus series velcro, it can increase 10% peel and shear strengths in    
 water
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>**test no BR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -524,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="H3" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.6"/>
@@ -588,16 +584,16 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -623,19 +619,16 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.6">

</xml_diff>